<commit_message>
dont hang infinitly in mqtt connection loop if server is unavailable
</commit_message>
<xml_diff>
--- a/nodemcu_V3/PowerConsumption.xlsx
+++ b/nodemcu_V3/PowerConsumption.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -408,7 +408,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,11 +444,11 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <f>C4*B4/3600</f>
-        <v>0.125</v>
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,11 +460,11 @@
         <v>300</v>
       </c>
       <c r="C5">
-        <v>2.8</v>
+        <v>0.02</v>
       </c>
       <c r="D5">
         <f>C5*B5/3600</f>
-        <v>0.23333333333333334</v>
+        <v>1.6666666666666668E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -491,13 +491,13 @@
       </c>
       <c r="B10">
         <f>(C4*B4+B5*C5)/B6</f>
-        <v>4.2295081967213113</v>
+        <v>1.1672131147540983</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14">
         <f>D15/1000</f>
-        <v>37.050491803278689</v>
+        <v>10.224786885245901</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,11 +508,11 @@
         <v>750</v>
       </c>
       <c r="C15">
-        <v>950</v>
+        <v>2450</v>
       </c>
       <c r="D15">
         <f>D16*B10</f>
-        <v>37050.491803278688</v>
+        <v>10224.786885245901</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,11 +521,11 @@
       </c>
       <c r="B16">
         <f>B15/$B$10</f>
-        <v>177.32558139534885</v>
+        <v>642.55617977528095</v>
       </c>
       <c r="C16">
         <f>C15/$B$10</f>
-        <v>224.6124031007752</v>
+        <v>2099.0168539325846</v>
       </c>
       <c r="D16">
         <f>D17*24</f>
@@ -538,11 +538,11 @@
       </c>
       <c r="B17">
         <f>B16/24</f>
-        <v>7.3885658914728687</v>
+        <v>26.773174157303373</v>
       </c>
       <c r="C17">
         <f>C16/24</f>
-        <v>9.3588501291989665</v>
+        <v>87.459035580524358</v>
       </c>
       <c r="D17">
         <v>365</v>

</xml_diff>